<commit_message>
Add describe function, mockup, and convert define to html.
</commit_message>
<xml_diff>
--- a/inst/template_spec_simplified.xlsx
+++ b/inst/template_spec_simplified.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="45" documentId="11_E8F9E9949DADA93E5E2004E2056B6066561B40AA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F5FBA9A-0FF9-47DE-95D4-6774A6017445}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="2" r:id="rId1"/>
@@ -347,7 +347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
@@ -1368,9 +1368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G618"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>